<commit_message>
added more to study recources section
</commit_message>
<xml_diff>
--- a/AI_ML Resources.xlsx
+++ b/AI_ML Resources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micintro/Desktop/Study Center Site/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micintro/Desktop/Web_Dev/Study Center Site/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2AB035-C2E0-254E-9274-240516249BCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA63F1-E9EC-2649-9B91-3A770B0FA1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" xr2:uid="{EF8DF5E4-6B9B-48D2-AD95-594758D9ACD4}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" xr2:uid="{EF8DF5E4-6B9B-48D2-AD95-594758D9ACD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="198">
   <si>
     <t>Group</t>
   </si>
@@ -616,6 +616,15 @@
   </si>
   <si>
     <t>https://medium.com/towards-artificial-intelligence/main-types-of-neural-networks-and-its-applications-tutorial-734480d7ec8e</t>
+  </si>
+  <si>
+    <t>Spark / Full sourse</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pEi-Ak5l00A&amp;list=PL3N9eeOlCrP5PfpYrP6YxMNtt5Hw27ZlO</t>
   </si>
 </sst>
 </file>
@@ -981,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FE980D-FD47-467A-A139-6C94C136C4A0}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1176,27 +1185,27 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>195</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>136</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1204,27 +1213,27 @@
         <v>136</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E17" t="s">
         <v>139</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E18" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1232,13 +1241,13 @@
         <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
         <v>152</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1246,13 +1255,13 @@
         <v>70</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20" t="s">
         <v>152</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1260,13 +1269,13 @@
         <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
         <v>152</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,66 +1283,63 @@
         <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22" t="s">
         <v>152</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>146</v>
+      <c r="G22" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>168</v>
+        <v>152</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>179</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>180</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>181</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="1"/>
-    </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1344,13 +1350,13 @@
         <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1361,13 +1367,13 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>86</v>
+      <c r="G29" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1378,13 +1384,13 @@
         <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>60</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1395,13 +1401,13 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
         <v>60</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1412,13 +1418,13 @@
         <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
         <v>60</v>
       </c>
-      <c r="G32" t="s">
-        <v>93</v>
+      <c r="G32" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
@@ -1429,13 +1435,13 @@
         <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
         <v>60</v>
       </c>
       <c r="G33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1446,13 +1452,13 @@
         <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
         <v>60</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>98</v>
+      <c r="G34" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
@@ -1463,13 +1469,13 @@
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1480,16 +1486,13 @@
         <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1500,13 +1503,16 @@
         <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E37" t="s">
         <v>60</v>
       </c>
+      <c r="F37" t="s">
+        <v>112</v>
+      </c>
       <c r="G37" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -1517,13 +1523,13 @@
         <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E38" t="s">
         <v>60</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -1534,30 +1540,30 @@
         <v>13</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
         <v>60</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>10</v>
       </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
         <v>60</v>
       </c>
-      <c r="F40" t="s">
-        <v>184</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -1565,7 +1571,7 @@
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
         <v>60</v>
@@ -1574,7 +1580,7 @@
         <v>184</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -1582,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E42" t="s">
         <v>60</v>
@@ -1591,7 +1597,7 @@
         <v>184</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
@@ -1599,7 +1605,7 @@
         <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
         <v>60</v>
@@ -1608,24 +1614,24 @@
         <v>184</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C44" t="s">
-        <v>81</v>
-      </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E44" t="s">
         <v>60</v>
       </c>
-      <c r="G44" t="s">
-        <v>91</v>
+      <c r="F44" t="s">
+        <v>184</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
@@ -1633,16 +1639,16 @@
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
         <v>60</v>
       </c>
       <c r="G45" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
@@ -1653,13 +1659,13 @@
         <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E46" t="s">
         <v>60</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>103</v>
+      <c r="G46" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
@@ -1670,58 +1676,61 @@
         <v>102</v>
       </c>
       <c r="D47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E47" t="s">
         <v>60</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>10</v>
       </c>
+      <c r="C48" t="s">
+        <v>102</v>
+      </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="E48" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>132</v>
+      <c r="G48" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="E49" t="s">
         <v>60</v>
       </c>
-      <c r="F49" t="s">
-        <v>184</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>69</v>
+      <c r="G49" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>60</v>
+      </c>
+      <c r="F50" t="s">
+        <v>184</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
@@ -1729,16 +1738,13 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E51" t="s">
-        <v>60</v>
-      </c>
-      <c r="F51" t="s">
-        <v>160</v>
-      </c>
-      <c r="G51" t="s">
-        <v>157</v>
+        <v>12</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.2">
@@ -1746,13 +1752,16 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E52" t="s">
         <v>60</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>162</v>
+      <c r="F52" t="s">
+        <v>160</v>
+      </c>
+      <c r="G52" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
@@ -1760,75 +1769,75 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E53" t="s">
         <v>60</v>
       </c>
-      <c r="F53" t="s">
-        <v>160</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>163</v>
+      <c r="G53" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="E54" t="s">
         <v>60</v>
       </c>
       <c r="F54" t="s">
-        <v>184</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>72</v>
+        <v>160</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" t="s">
-        <v>20</v>
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>71</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>60</v>
+      </c>
+      <c r="F55" t="s">
+        <v>184</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>120</v>
-      </c>
-      <c r="D56" t="s">
-        <v>122</v>
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>60</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>121</v>
+        <v>12</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="D57" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="E57" t="s">
-        <v>41</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
@@ -1836,13 +1845,13 @@
         <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E58" t="s">
         <v>41</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
@@ -1850,70 +1859,67 @@
         <v>34</v>
       </c>
       <c r="D59" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>125</v>
-      </c>
-      <c r="C60" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="E60" t="s">
-        <v>60</v>
-      </c>
-      <c r="F60" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>129</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>153</v>
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>126</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="E61" t="s">
-        <v>156</v>
+        <v>60</v>
       </c>
       <c r="F61" t="s">
         <v>128</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>153</v>
       </c>
-      <c r="C62" t="s">
-        <v>169</v>
-      </c>
       <c r="D62" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="F62" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>153</v>
       </c>
@@ -1921,13 +1927,13 @@
         <v>169</v>
       </c>
       <c r="D63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E63" t="s">
         <v>174</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
@@ -1938,13 +1944,13 @@
         <v>169</v>
       </c>
       <c r="D64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E64" t="s">
         <v>174</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
@@ -1955,44 +1961,47 @@
         <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E65" t="s">
         <v>174</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>186</v>
+        <v>153</v>
       </c>
       <c r="C66" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E66" t="s">
-        <v>60</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>70</v>
+        <v>186</v>
+      </c>
+      <c r="C67" t="s">
+        <v>187</v>
       </c>
       <c r="D67" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E67" t="s">
         <v>60</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
@@ -2000,47 +2009,44 @@
         <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>71</v>
+        <v>185</v>
       </c>
       <c r="E68" t="s">
         <v>60</v>
       </c>
-      <c r="F68" t="s">
-        <v>184</v>
-      </c>
       <c r="G68" s="1" t="s">
-        <v>72</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>192</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="E69" t="s">
         <v>60</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>194</v>
+      <c r="F69" t="s">
+        <v>184</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>74</v>
+        <v>192</v>
       </c>
       <c r="D70" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
       <c r="E70" t="s">
-        <v>24</v>
-      </c>
-      <c r="F70" t="s">
-        <v>25</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.2">
@@ -2048,7 +2054,7 @@
         <v>74</v>
       </c>
       <c r="D71" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="E71" t="s">
         <v>24</v>
@@ -2057,7 +2063,7 @@
         <v>25</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
@@ -2065,13 +2071,16 @@
         <v>74</v>
       </c>
       <c r="D72" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E72" t="s">
-        <v>60</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>82</v>
+        <v>24</v>
+      </c>
+      <c r="F72" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.2">
@@ -2079,16 +2088,13 @@
         <v>74</v>
       </c>
       <c r="D73" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E73" t="s">
         <v>60</v>
       </c>
-      <c r="F73" t="s">
-        <v>184</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>73</v>
+      <c r="G73" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.2">
@@ -2096,7 +2102,7 @@
         <v>74</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E74" t="s">
         <v>60</v>
@@ -2105,7 +2111,7 @@
         <v>184</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.2">
@@ -2113,16 +2119,16 @@
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="E75" t="s">
         <v>60</v>
       </c>
       <c r="F75" t="s">
-        <v>115</v>
-      </c>
-      <c r="G75" t="s">
-        <v>113</v>
+        <v>184</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.2">
@@ -2130,13 +2136,16 @@
         <v>74</v>
       </c>
       <c r="D76" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E76" t="s">
         <v>60</v>
       </c>
+      <c r="F76" t="s">
+        <v>115</v>
+      </c>
       <c r="G76" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.2">
@@ -2144,30 +2153,27 @@
         <v>74</v>
       </c>
       <c r="D77" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E77" t="s">
         <v>60</v>
       </c>
-      <c r="G77" s="1" t="s">
-        <v>135</v>
+      <c r="G77" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>74</v>
       </c>
-      <c r="C78" t="s">
-        <v>20</v>
-      </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="E78" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.2">
@@ -2175,81 +2181,99 @@
         <v>74</v>
       </c>
       <c r="C79" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" t="s">
+        <v>165</v>
+      </c>
+      <c r="E79" t="s">
+        <v>152</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" t="s">
         <v>187</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>190</v>
       </c>
-      <c r="E79" t="s">
-        <v>60</v>
-      </c>
-      <c r="G79" s="2" t="s">
+      <c r="E80" t="s">
+        <v>60</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>191</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G50" r:id="rId1" xr:uid="{0CAD79C3-0EA8-4CAD-AB45-B36223618E97}"/>
-    <hyperlink ref="G55" r:id="rId2" xr:uid="{7F7AE2A4-9136-42CC-83ED-21886096DA0E}"/>
-    <hyperlink ref="G27" r:id="rId3" xr:uid="{57C978A8-E98C-49D5-A1FF-8E88C2BFB90A}"/>
+    <hyperlink ref="G51" r:id="rId1" xr:uid="{0CAD79C3-0EA8-4CAD-AB45-B36223618E97}"/>
+    <hyperlink ref="G56" r:id="rId2" xr:uid="{7F7AE2A4-9136-42CC-83ED-21886096DA0E}"/>
+    <hyperlink ref="G28" r:id="rId3" xr:uid="{57C978A8-E98C-49D5-A1FF-8E88C2BFB90A}"/>
     <hyperlink ref="G6" r:id="rId4" xr:uid="{D06FC7AF-CD7D-4895-8BA7-0E05271E664A}"/>
     <hyperlink ref="G3" r:id="rId5" display="https://cisgov.sharepoint.com/teams/Attain_MDASII_BiometricsTeams/Shared Documents/Forms/AllItems.aspx?FolderCTID=0x012000FC6993A99A341546AC9887925E64AF16&amp;id=%2Fteams%2FAttain%5FMDASII%5FBiometricsTeams%2FShared%20Documents%2FMDAS%2DAI%2FClassification%20%2D%20COA%20work%20update%20and%20info%20exchange%2D20200526%201930%2D1%2Emp4&amp;parent=%2Fteams%2FAttain%5FMDASII%5FBiometricsTeams%2FShared%20Documents%2FMDAS%2DAI" xr:uid="{75710CF6-25D1-49F6-B8EF-537188880DDD}"/>
-    <hyperlink ref="G57" r:id="rId6" display="https://towardsdatascience.com/my-10-recommendations-after-getting-the-databricks-certification-for-apache-spark-53cd3690073" xr:uid="{086D5F3E-4EE9-4BF9-B8BF-822627DE14C7}"/>
-    <hyperlink ref="G58" r:id="rId7" display="https://docs.databricks.com/notebooks/github-version-control.html" xr:uid="{A662F839-22B2-4985-BC03-34F85362FAC7}"/>
-    <hyperlink ref="G59" r:id="rId8" display="https://docs.databricks.com/index.html" xr:uid="{4C96A0D3-EFCF-41F0-BC43-D2FE9CED876F}"/>
+    <hyperlink ref="G58" r:id="rId6" display="https://towardsdatascience.com/my-10-recommendations-after-getting-the-databricks-certification-for-apache-spark-53cd3690073" xr:uid="{086D5F3E-4EE9-4BF9-B8BF-822627DE14C7}"/>
+    <hyperlink ref="G59" r:id="rId7" display="https://docs.databricks.com/notebooks/github-version-control.html" xr:uid="{A662F839-22B2-4985-BC03-34F85362FAC7}"/>
+    <hyperlink ref="G60" r:id="rId8" display="https://docs.databricks.com/index.html" xr:uid="{4C96A0D3-EFCF-41F0-BC43-D2FE9CED876F}"/>
     <hyperlink ref="G10" r:id="rId9" display="https://maestro.dhs.gov/confluence/display/DBIS/DevOps+Practices+for+Databricks" xr:uid="{4C61339A-1DE0-4436-975E-00AD59B2ED01}"/>
     <hyperlink ref="G11" r:id="rId10" display="https://maestro.dhs.gov/confluence/pages/viewpage.action?pageId=203866752" xr:uid="{2EA7A5DD-C520-44F5-A4C8-2223D1925C31}"/>
     <hyperlink ref="G12" r:id="rId11" display="https://maestro.dhs.gov/confluence/display/DBIS/DevOPS+Effort+-+Databricks+Pipeline" xr:uid="{54C2D094-36D1-4009-9052-09295F4B7033}"/>
     <hyperlink ref="G13" r:id="rId12" display="https://maestro.dhs.gov/confluence/display/DBIS/Databricks+Pipeline+Setup+and+Description" xr:uid="{57C5E6D2-987A-4986-A3BF-C286E4A506E8}"/>
     <hyperlink ref="G14" r:id="rId13" display="https://maestro.dhs.gov/confluence/pages/viewpage.action?pageId=126321699" xr:uid="{C40F01DC-8695-49C2-AF55-2DEBD493722C}"/>
-    <hyperlink ref="G15" r:id="rId14" display="https://maestro.dhs.gov/confluence/display/DBIS/Databricks+Documentaton" xr:uid="{22569694-38FF-4F9B-BEC4-4AED2C58D499}"/>
+    <hyperlink ref="G16" r:id="rId14" display="https://maestro.dhs.gov/confluence/display/DBIS/Databricks+Documentaton" xr:uid="{22569694-38FF-4F9B-BEC4-4AED2C58D499}"/>
     <hyperlink ref="G7" r:id="rId15" xr:uid="{2C92E94F-5B79-4B89-AFB6-E19BFFAA7209}"/>
     <hyperlink ref="G8" r:id="rId16" display="https://cisgov.sharepoint.com/:w:/r/teams/Attain_MDASII_BiometricsTeams/_layouts/15/Doc.aspx?sourcedoc=%7B5B38F1D9-F3C7-431A-B8CF-FB5BB190C576%7D&amp;file=Setting%20up%20Jupyter%20Notebook%20on%20EC2%20and%20accessing%20from%20localhost.docx&amp;action=default&amp;mobileredirect=true" xr:uid="{51B62675-1752-417D-BDF4-F663D9BA8E25}"/>
-    <hyperlink ref="G41" r:id="rId17" display="https://github.com/micintron/Documents/blob/master/AWS Data Storage Overview.docx" xr:uid="{B68D6F46-88DF-4FC7-B144-06BBDA71DB5C}"/>
-    <hyperlink ref="G42" r:id="rId18" display="https://github.com/micintron/Documents/blob/master/AWS Cloud Practitioners   Essentials.docx" xr:uid="{8BC7AAEA-0E6A-4E00-9CAE-3174596D824B}"/>
-    <hyperlink ref="G43" r:id="rId19" xr:uid="{F1D60058-044E-4499-806B-55DC47985806}"/>
-    <hyperlink ref="G49" r:id="rId20" xr:uid="{0E46FFE5-5C12-4CE4-8DC5-BF533D3B47CA}"/>
-    <hyperlink ref="G54" r:id="rId21" xr:uid="{CA8436B7-36B0-49B3-A878-19128DEA0F21}"/>
-    <hyperlink ref="G29" r:id="rId22" display="about:blank" xr:uid="{4A686B63-5E15-4E40-9373-162E0C2459B8}"/>
-    <hyperlink ref="G31" r:id="rId23" display="about:blank" xr:uid="{1196AD08-C228-4B58-9CBE-7DBEC890CA84}"/>
+    <hyperlink ref="G42" r:id="rId17" display="https://github.com/micintron/Documents/blob/master/AWS Data Storage Overview.docx" xr:uid="{B68D6F46-88DF-4FC7-B144-06BBDA71DB5C}"/>
+    <hyperlink ref="G43" r:id="rId18" display="https://github.com/micintron/Documents/blob/master/AWS Cloud Practitioners   Essentials.docx" xr:uid="{8BC7AAEA-0E6A-4E00-9CAE-3174596D824B}"/>
+    <hyperlink ref="G44" r:id="rId19" xr:uid="{F1D60058-044E-4499-806B-55DC47985806}"/>
+    <hyperlink ref="G50" r:id="rId20" xr:uid="{0E46FFE5-5C12-4CE4-8DC5-BF533D3B47CA}"/>
+    <hyperlink ref="G55" r:id="rId21" xr:uid="{CA8436B7-36B0-49B3-A878-19128DEA0F21}"/>
+    <hyperlink ref="G30" r:id="rId22" display="about:blank" xr:uid="{4A686B63-5E15-4E40-9373-162E0C2459B8}"/>
+    <hyperlink ref="G32" r:id="rId23" display="about:blank" xr:uid="{1196AD08-C228-4B58-9CBE-7DBEC890CA84}"/>
     <hyperlink ref="G9" r:id="rId24" display="about:blank" xr:uid="{CC6CAB7E-A344-4532-AF5E-A13F191B5D27}"/>
-    <hyperlink ref="G34" r:id="rId25" display="about:blank" xr:uid="{CC55FB6F-9C12-4392-BF31-BEDF771B7025}"/>
-    <hyperlink ref="G46" r:id="rId26" display="about:blank" xr:uid="{C3D6A980-8EEF-4CBA-A54F-43855BC53C76}"/>
-    <hyperlink ref="G40" r:id="rId27" display="https://github.com/micintron/Documents/blob/master/AWS ML tools overview.docx" xr:uid="{BA9088D0-5057-4A0C-A8F2-E5E212BF8379}"/>
-    <hyperlink ref="G56" r:id="rId28" display="about:blank" xr:uid="{69443572-974F-488E-90A6-C08821ED3E9E}"/>
-    <hyperlink ref="G60" r:id="rId29" xr:uid="{166BA7BD-20AD-4B4A-BA9C-50545A1074D4}"/>
-    <hyperlink ref="G39" r:id="rId30" xr:uid="{D3EB7798-F8FD-4978-ACFE-76A1EEDFF240}"/>
-    <hyperlink ref="G48" r:id="rId31" xr:uid="{B413A625-D279-4AA1-8E28-0A21DBF4329D}"/>
-    <hyperlink ref="G16" r:id="rId32" xr:uid="{0DDB0BC0-D06D-4F12-AD4D-A251745BF131}"/>
-    <hyperlink ref="G17" r:id="rId33" xr:uid="{FB403D98-1863-45F5-A185-0827CBFFCA7F}"/>
-    <hyperlink ref="G18" r:id="rId34" xr:uid="{83AE4B60-1DD9-4453-B5B8-0AF7BF76DB50}"/>
-    <hyperlink ref="G19" r:id="rId35" xr:uid="{981A7D26-D01D-4BC7-B8A6-0980DB2DAF99}"/>
-    <hyperlink ref="G20" r:id="rId36" display="https://maestro.dhs.gov/jira/secure/RapidBoard.jspa?rapidView=5945&amp;projectKey=MATRIX&amp;view=planning&amp;issueLimit=100" xr:uid="{5D701A2E-4CA5-4C76-A516-F824B5C090E9}"/>
-    <hyperlink ref="G21" r:id="rId37" xr:uid="{8C784ED6-12E7-46B4-8D99-1D615030EFC4}"/>
-    <hyperlink ref="G22" r:id="rId38" xr:uid="{8640520F-9A81-484F-A257-56066BCCE5A7}"/>
-    <hyperlink ref="G61" r:id="rId39" xr:uid="{29F51B9E-3323-4AB7-BE8E-5F0123436910}"/>
-    <hyperlink ref="G52" r:id="rId40" xr:uid="{2AEBA06B-2CB1-4D60-9A4A-80CC72E4955D}"/>
-    <hyperlink ref="G53" r:id="rId41" display="https://www.youtube.com/watch?v=ZkPQtjETrBw" xr:uid="{C74F4A7F-0858-4F33-8D6E-6D1F83BDF6B0}"/>
-    <hyperlink ref="G23" r:id="rId42" xr:uid="{44A3A124-C919-4416-9198-77EED8CA97C6}"/>
-    <hyperlink ref="G62" r:id="rId43" xr:uid="{3566BF08-10AA-4A9E-A03B-0B28E522F524}"/>
-    <hyperlink ref="G63" r:id="rId44" xr:uid="{CC40B5CE-3081-4B96-B757-946E16D3F043}"/>
-    <hyperlink ref="G64" r:id="rId45" xr:uid="{33CB3B7D-62D3-4533-9B51-A4976CCEDEDF}"/>
-    <hyperlink ref="G65" r:id="rId46" xr:uid="{B89978CF-7B7A-4E3D-B585-CCF1508B0039}"/>
-    <hyperlink ref="G24" r:id="rId47" xr:uid="{26133D2D-578C-434B-8DD5-B4F7331AF648}"/>
-    <hyperlink ref="G66" r:id="rId48" xr:uid="{F8B66884-987E-49B1-905F-452D1F79B85C}"/>
-    <hyperlink ref="G68" r:id="rId49" xr:uid="{29A41225-CF28-4491-831B-F13DA87B34E3}"/>
-    <hyperlink ref="G67" r:id="rId50" xr:uid="{B5E623CA-8372-4F6A-89D9-2FE78FEA429B}"/>
-    <hyperlink ref="G69" r:id="rId51" xr:uid="{C6378766-544D-4AB1-98C5-C12CD26CDD41}"/>
-    <hyperlink ref="G70" r:id="rId52" xr:uid="{5287165F-4D25-7E4C-BE61-AB57B83BDD78}"/>
-    <hyperlink ref="G71" r:id="rId53" xr:uid="{289DBC1E-68E4-D548-B8D0-682048E2A7BC}"/>
-    <hyperlink ref="G72" r:id="rId54" display="about:blank" xr:uid="{547AA79B-0D80-4248-A131-1BAEC2084B23}"/>
-    <hyperlink ref="G73" r:id="rId55" xr:uid="{8826E778-6CE9-9A49-8C35-432ACD2DFA88}"/>
-    <hyperlink ref="G74" r:id="rId56" xr:uid="{B608B51B-9289-7A4A-A6DF-B830F1A2211F}"/>
-    <hyperlink ref="G77" r:id="rId57" xr:uid="{16E8F3D8-5C34-7E45-81B3-920D2E6BD91A}"/>
-    <hyperlink ref="G78" r:id="rId58" xr:uid="{97DE4675-2D67-D548-B7F7-01F71D063E4B}"/>
-    <hyperlink ref="G79" r:id="rId59" xr:uid="{CFE46A76-6BF6-BC4B-A577-4DF8B60B303A}"/>
+    <hyperlink ref="G35" r:id="rId25" display="about:blank" xr:uid="{CC55FB6F-9C12-4392-BF31-BEDF771B7025}"/>
+    <hyperlink ref="G47" r:id="rId26" display="about:blank" xr:uid="{C3D6A980-8EEF-4CBA-A54F-43855BC53C76}"/>
+    <hyperlink ref="G41" r:id="rId27" display="https://github.com/micintron/Documents/blob/master/AWS ML tools overview.docx" xr:uid="{BA9088D0-5057-4A0C-A8F2-E5E212BF8379}"/>
+    <hyperlink ref="G57" r:id="rId28" display="about:blank" xr:uid="{69443572-974F-488E-90A6-C08821ED3E9E}"/>
+    <hyperlink ref="G61" r:id="rId29" xr:uid="{166BA7BD-20AD-4B4A-BA9C-50545A1074D4}"/>
+    <hyperlink ref="G40" r:id="rId30" xr:uid="{D3EB7798-F8FD-4978-ACFE-76A1EEDFF240}"/>
+    <hyperlink ref="G49" r:id="rId31" xr:uid="{B413A625-D279-4AA1-8E28-0A21DBF4329D}"/>
+    <hyperlink ref="G17" r:id="rId32" xr:uid="{0DDB0BC0-D06D-4F12-AD4D-A251745BF131}"/>
+    <hyperlink ref="G18" r:id="rId33" xr:uid="{FB403D98-1863-45F5-A185-0827CBFFCA7F}"/>
+    <hyperlink ref="G19" r:id="rId34" xr:uid="{83AE4B60-1DD9-4453-B5B8-0AF7BF76DB50}"/>
+    <hyperlink ref="G20" r:id="rId35" xr:uid="{981A7D26-D01D-4BC7-B8A6-0980DB2DAF99}"/>
+    <hyperlink ref="G21" r:id="rId36" display="https://maestro.dhs.gov/jira/secure/RapidBoard.jspa?rapidView=5945&amp;projectKey=MATRIX&amp;view=planning&amp;issueLimit=100" xr:uid="{5D701A2E-4CA5-4C76-A516-F824B5C090E9}"/>
+    <hyperlink ref="G22" r:id="rId37" xr:uid="{8C784ED6-12E7-46B4-8D99-1D615030EFC4}"/>
+    <hyperlink ref="G23" r:id="rId38" xr:uid="{8640520F-9A81-484F-A257-56066BCCE5A7}"/>
+    <hyperlink ref="G62" r:id="rId39" xr:uid="{29F51B9E-3323-4AB7-BE8E-5F0123436910}"/>
+    <hyperlink ref="G53" r:id="rId40" xr:uid="{2AEBA06B-2CB1-4D60-9A4A-80CC72E4955D}"/>
+    <hyperlink ref="G54" r:id="rId41" display="https://www.youtube.com/watch?v=ZkPQtjETrBw" xr:uid="{C74F4A7F-0858-4F33-8D6E-6D1F83BDF6B0}"/>
+    <hyperlink ref="G24" r:id="rId42" xr:uid="{44A3A124-C919-4416-9198-77EED8CA97C6}"/>
+    <hyperlink ref="G63" r:id="rId43" xr:uid="{3566BF08-10AA-4A9E-A03B-0B28E522F524}"/>
+    <hyperlink ref="G64" r:id="rId44" xr:uid="{CC40B5CE-3081-4B96-B757-946E16D3F043}"/>
+    <hyperlink ref="G65" r:id="rId45" xr:uid="{33CB3B7D-62D3-4533-9B51-A4976CCEDEDF}"/>
+    <hyperlink ref="G66" r:id="rId46" xr:uid="{B89978CF-7B7A-4E3D-B585-CCF1508B0039}"/>
+    <hyperlink ref="G25" r:id="rId47" xr:uid="{26133D2D-578C-434B-8DD5-B4F7331AF648}"/>
+    <hyperlink ref="G67" r:id="rId48" xr:uid="{F8B66884-987E-49B1-905F-452D1F79B85C}"/>
+    <hyperlink ref="G69" r:id="rId49" xr:uid="{29A41225-CF28-4491-831B-F13DA87B34E3}"/>
+    <hyperlink ref="G68" r:id="rId50" xr:uid="{B5E623CA-8372-4F6A-89D9-2FE78FEA429B}"/>
+    <hyperlink ref="G70" r:id="rId51" xr:uid="{C6378766-544D-4AB1-98C5-C12CD26CDD41}"/>
+    <hyperlink ref="G71" r:id="rId52" xr:uid="{5287165F-4D25-7E4C-BE61-AB57B83BDD78}"/>
+    <hyperlink ref="G72" r:id="rId53" xr:uid="{289DBC1E-68E4-D548-B8D0-682048E2A7BC}"/>
+    <hyperlink ref="G73" r:id="rId54" display="about:blank" xr:uid="{547AA79B-0D80-4248-A131-1BAEC2084B23}"/>
+    <hyperlink ref="G74" r:id="rId55" xr:uid="{8826E778-6CE9-9A49-8C35-432ACD2DFA88}"/>
+    <hyperlink ref="G75" r:id="rId56" xr:uid="{B608B51B-9289-7A4A-A6DF-B830F1A2211F}"/>
+    <hyperlink ref="G78" r:id="rId57" xr:uid="{16E8F3D8-5C34-7E45-81B3-920D2E6BD91A}"/>
+    <hyperlink ref="G79" r:id="rId58" xr:uid="{97DE4675-2D67-D548-B7F7-01F71D063E4B}"/>
+    <hyperlink ref="G80" r:id="rId59" xr:uid="{CFE46A76-6BF6-BC4B-A577-4DF8B60B303A}"/>
+    <hyperlink ref="G15" r:id="rId60" xr:uid="{D7F2E8DD-9644-C843-B18A-1F4177CAD15F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId60"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId61"/>
 </worksheet>
 </file>
</xml_diff>